<commit_message>
completed mid project presentation
</commit_message>
<xml_diff>
--- a/proposal/presentation/times.xlsx
+++ b/proposal/presentation/times.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26057" windowHeight="14500" activeTab="1"/>
+    <workbookView windowWidth="31241" windowHeight="14500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,9 +104,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -118,32 +118,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -157,24 +155,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -188,9 +170,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -198,7 +187,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,29 +217,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,15 +246,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -295,7 +295,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,7 +343,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -319,13 +433,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -337,55 +463,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -397,85 +475,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -500,45 +500,6 @@
       </top>
       <bottom style="thin">
         <color auto="true"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -596,6 +557,45 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -606,118 +606,118 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -726,28 +726,28 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -10451,8 +10451,8 @@
   <sheetPr/>
   <dimension ref="B2:T84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J9" workbookViewId="0">
-      <selection activeCell="U34" sqref="U34"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="G37" workbookViewId="0">
+      <selection activeCell="U74" sqref="U74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
organized files in appropriate directories for submission
</commit_message>
<xml_diff>
--- a/proposal/presentation/times.xlsx
+++ b/proposal/presentation/times.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26057" windowHeight="14500" tabRatio="720" activeTab="4"/>
+    <workbookView windowWidth="31241" windowHeight="14500" tabRatio="720" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -186,11 +186,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.00_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -198,6 +198,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -210,7 +217,53 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -224,14 +277,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,7 +308,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,24 +322,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -286,60 +339,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -378,6 +378,126 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -390,13 +510,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,127 +546,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,25 +558,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -661,6 +661,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -675,185 +684,170 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="9" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
@@ -3383,10 +3377,10 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="" altLang="en-US"/>
+                  <a:rPr lang="en-US" altLang="en-US"/>
                   <a:t>Percentage Time Saved (Local - Distributed)/Local</a:t>
                 </a:r>
-                <a:endParaRPr lang="" altLang="en-US"/>
+                <a:endParaRPr lang="en-US" altLang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3548,10 +3542,10 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="" altLang="en-US"/>
+              <a:rPr lang="en-US" altLang="en-US"/>
               <a:t>Overhead of 1 Worker Failure at Different Stages</a:t>
             </a:r>
-            <a:endParaRPr lang="" altLang="en-US"/>
+            <a:endParaRPr lang="en-US" altLang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3812,10 +3806,10 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="" altLang="en-US"/>
+                  <a:rPr lang="en-US" altLang="en-US"/>
                   <a:t>Node Failure at Different Points</a:t>
                 </a:r>
-                <a:endParaRPr lang="" altLang="en-US"/>
+                <a:endParaRPr lang="en-US" altLang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3919,10 +3913,10 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="" altLang="en-US"/>
+                  <a:rPr lang="en-US" altLang="en-US"/>
                   <a:t>Time (s)</a:t>
                 </a:r>
-                <a:endParaRPr lang="" altLang="en-US"/>
+                <a:endParaRPr lang="en-US" altLang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4048,10 +4042,10 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="" altLang="en-US"/>
+              <a:rPr lang="en-US" altLang="en-US"/>
               <a:t>Caching Vs. No Caching</a:t>
             </a:r>
-            <a:endParaRPr lang="" altLang="en-US"/>
+            <a:endParaRPr lang="en-US" altLang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -4259,6 +4253,7 @@
         <c:axId val="305672465"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="false"/>
         <c:axPos val="l"/>
@@ -4296,10 +4291,10 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="" altLang="en-US"/>
+                  <a:rPr lang="en-US" altLang="en-US"/>
                   <a:t>Time (s)</a:t>
                 </a:r>
-                <a:endParaRPr lang="" altLang="en-US"/>
+                <a:endParaRPr lang="en-US" altLang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -17270,7 +17265,7 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:5">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -17284,7 +17279,7 @@
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="18" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1">
@@ -17298,7 +17293,7 @@
       </c>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="18" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1">
@@ -17312,7 +17307,7 @@
       </c>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="18" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1">
@@ -17326,7 +17321,7 @@
       </c>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1">
@@ -17340,10 +17335,10 @@
       </c>
     </row>
     <row r="9" spans="2:2">
-      <c r="B9" s="20"/>
+      <c r="B9" s="18"/>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="1">
@@ -17357,7 +17352,7 @@
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1">
@@ -17371,7 +17366,7 @@
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="1">
@@ -17385,7 +17380,7 @@
       </c>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="1">
@@ -17435,30 +17430,30 @@
       <c r="G3" s="1"/>
     </row>
     <row r="5" ht="30" customHeight="true" spans="2:20">
-      <c r="B5" s="8"/>
-      <c r="C5" s="9" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9" t="s">
+      <c r="G5" s="7"/>
+      <c r="H5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="M5" s="1" t="s">
@@ -17473,62 +17468,62 @@
       <c r="T5" s="1"/>
     </row>
     <row r="6" s="1" customFormat="true" spans="2:11">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <v>0.021826703</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>0.499183426</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="9">
         <v>0.00255803</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="9">
         <v>0.127816207</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="11">
+      <c r="G6" s="15"/>
+      <c r="H6" s="9">
         <v>0.000218114</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="9">
         <v>0.021962754</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="9">
         <v>0.49857035</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="9">
         <v>0.253367378</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="true" spans="2:13">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <v>0.022173456</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="9">
         <v>0.488145022</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="9">
         <v>0.004626178</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="9">
         <v>0.133414299</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="11">
+      <c r="G7" s="15"/>
+      <c r="H7" s="9">
         <v>0.000266863</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="9">
         <v>0.02193585</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="9">
         <v>0.487887168</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="9">
         <v>0.266928699</v>
       </c>
       <c r="M7" s="1" t="s">
@@ -17536,112 +17531,112 @@
       </c>
     </row>
     <row r="8" s="1" customFormat="true" spans="2:11">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>0.022503715</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <v>0.495740048</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="9">
         <v>0.004269732</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="9">
         <v>0.126129945</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="11">
+      <c r="G8" s="15"/>
+      <c r="H8" s="9">
         <v>0.000217581</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="9">
         <v>0.022162441</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="9">
         <v>0.495609731</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="9">
         <v>0.257223187</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="true" spans="2:11">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="8">
         <f>AVERAGE(C6:C8)</f>
         <v>0.022167958</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="8">
         <f>AVERAGE(D6:D8)</f>
         <v>0.494356165333333</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="8">
         <f>AVERAGE(E6:E8)</f>
         <v>0.00381798</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="8">
         <f>AVERAGE(F6:F8)</f>
         <v>0.129120150333333</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="10">
+      <c r="G9" s="16"/>
+      <c r="H9" s="8">
         <f>AVERAGE(H6:H8)</f>
         <v>0.000234186</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="8">
         <f>AVERAGE(I6:I8)</f>
         <v>0.0220203483333333</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="8">
         <f>AVERAGE(J6:J8)</f>
         <v>0.494022416333333</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="8">
         <f>AVERAGE(K6:K8)</f>
         <v>0.259173088</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="true" spans="2:11">
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
     </row>
     <row r="11" s="1" customFormat="true" spans="2:13">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="9">
         <v>0.022453049</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="9">
         <v>1.599032148</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="9">
         <v>0.071305635</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="9">
         <v>0.651175015</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="11">
+      <c r="G11" s="15"/>
+      <c r="H11" s="9">
         <v>0.000236792</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="9">
         <v>0.022274124</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="9">
         <v>1.598095176</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="9">
         <v>0.877651263</v>
       </c>
       <c r="M11" s="1" t="s">
@@ -17649,379 +17644,379 @@
       </c>
     </row>
     <row r="12" s="1" customFormat="true" spans="2:11">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="9">
         <v>0.022483319</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="9">
         <v>1.744556673</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="9">
         <v>0.01435518</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="9">
         <v>0.458791061</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="11">
+      <c r="G12" s="15"/>
+      <c r="H12" s="9">
         <v>0.000225654</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="9">
         <v>0.022179012</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="9">
         <v>1.744543638</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="9">
         <v>0.811443426</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="true" spans="2:11">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="9">
         <v>0.022769933</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="9">
         <v>1.583520056</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="9">
         <v>0.018134454</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="9">
         <v>0.493393134</v>
       </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="11">
+      <c r="G13" s="15"/>
+      <c r="H13" s="9">
         <v>0.000231103</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="9">
         <v>0.021755327</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="9">
         <v>1.583508261</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="9">
         <v>0.816626041</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="true" spans="2:11">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="8">
         <f>AVERAGE(C11:C13)</f>
         <v>0.022568767</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="8">
         <f t="shared" ref="D14:K14" si="0">AVERAGE(D11:D13)</f>
         <v>1.64236962566667</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="8">
         <f t="shared" si="0"/>
         <v>0.034598423</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="8">
         <f t="shared" si="0"/>
         <v>0.53445307</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10">
+      <c r="G14" s="8"/>
+      <c r="H14" s="8">
         <f t="shared" si="0"/>
         <v>0.000231183</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="8">
         <f t="shared" si="0"/>
         <v>0.0220694876666667</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="8">
         <f t="shared" si="0"/>
         <v>1.642049025</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="8">
         <f t="shared" si="0"/>
         <v>0.835240243333333</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="true" spans="2:11">
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" s="1" customFormat="true" spans="2:11">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="9">
         <v>0.024287961</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="9">
         <v>6.111266277</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="9">
         <v>0.173323656</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="9">
         <v>2.554161888</v>
       </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="11">
+      <c r="G16" s="15"/>
+      <c r="H16" s="9">
         <v>0.00026722</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="9">
         <v>0.023317513</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="9">
         <v>6.11107611</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="9">
         <v>3.100384348</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="true" spans="2:11">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="9">
         <v>0.02616225</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="9">
         <v>5.908088209</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="9">
         <v>0.173807943</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="9">
         <v>2.802237456</v>
       </c>
-      <c r="G17" s="17"/>
-      <c r="H17" s="11">
+      <c r="G17" s="15"/>
+      <c r="H17" s="9">
         <v>0.00021662</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="9">
         <v>0.025873341</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="9">
         <v>5.907915483</v>
       </c>
-      <c r="K17" s="11">
+      <c r="K17" s="9">
         <v>3.318008016</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="true" spans="2:11">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="9">
         <v>0.024348226</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="9">
         <v>6.720109741</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="9">
         <v>0.190167505</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="9">
         <v>2.713328619</v>
       </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="11">
+      <c r="G18" s="15"/>
+      <c r="H18" s="9">
         <v>0.00021383</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="9">
         <v>0.024037283</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J18" s="9">
         <v>6.720032964</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="9">
         <v>3.136473807</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="true" spans="2:11">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="8">
         <f>AVERAGE(C16:C18)</f>
         <v>0.0249328123333333</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="8">
         <f t="shared" ref="D19:K19" si="1">AVERAGE(D16:D18)</f>
         <v>6.24648807566667</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="8">
         <f t="shared" si="1"/>
         <v>0.179099701333333</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="8">
         <f t="shared" si="1"/>
         <v>2.689909321</v>
       </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10">
+      <c r="G19" s="8"/>
+      <c r="H19" s="8">
         <f t="shared" si="1"/>
         <v>0.000232556666666667</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="8">
         <f t="shared" si="1"/>
         <v>0.024409379</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="8">
         <f t="shared" si="1"/>
         <v>6.246341519</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="8">
         <f t="shared" si="1"/>
         <v>3.18495539033333</v>
       </c>
     </row>
     <row r="20" s="1" customFormat="true" spans="2:11">
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
     </row>
     <row r="21" s="1" customFormat="true" spans="2:11">
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="9">
         <v>0.02258302</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="9">
         <v>28.108442275</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="9">
         <v>2.263017355</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="9">
         <v>10.970606217</v>
       </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="11">
+      <c r="G21" s="15"/>
+      <c r="H21" s="9">
         <v>0.000221173</v>
       </c>
-      <c r="I21" s="11">
+      <c r="I21" s="9">
         <v>0.021966953</v>
       </c>
-      <c r="J21" s="11">
+      <c r="J21" s="9">
         <v>28.108477382</v>
       </c>
-      <c r="K21" s="11">
+      <c r="K21" s="9">
         <v>13.715560908</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="true" spans="2:11">
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="9">
         <v>0.022233708</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="9">
         <v>24.328802973</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="9">
         <v>2.251599524</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="9">
         <v>10.977483019</v>
       </c>
-      <c r="G22" s="17"/>
-      <c r="H22" s="11">
+      <c r="G22" s="15"/>
+      <c r="H22" s="9">
         <v>0.000236763</v>
       </c>
-      <c r="I22" s="11">
+      <c r="I22" s="9">
         <v>0.021786162</v>
       </c>
-      <c r="J22" s="11">
+      <c r="J22" s="9">
         <v>24.328688019</v>
       </c>
-      <c r="K22" s="11">
+      <c r="K22" s="9">
         <v>13.656840633</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="true" spans="2:11">
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="9">
         <v>0.022512853</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="9">
         <v>27.901384228</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="9">
         <v>2.166321529</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="9">
         <v>11.001965338</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="11">
+      <c r="G23" s="15"/>
+      <c r="H23" s="9">
         <v>0.000220294</v>
       </c>
-      <c r="I23" s="11">
+      <c r="I23" s="9">
         <v>0.022195933</v>
       </c>
-      <c r="J23" s="11">
+      <c r="J23" s="9">
         <v>27.901214684</v>
       </c>
-      <c r="K23" s="11">
+      <c r="K23" s="9">
         <v>13.634285811</v>
       </c>
     </row>
     <row r="24" spans="2:11">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="8">
         <f>AVERAGE(C21:C23)</f>
         <v>0.0224431936666667</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="8">
         <f t="shared" ref="D24:K24" si="2">AVERAGE(D21:D23)</f>
         <v>26.7795431586667</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="8">
         <f t="shared" si="2"/>
         <v>2.22697946933333</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24" s="8">
         <f t="shared" si="2"/>
         <v>10.9833515246667</v>
       </c>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10">
+      <c r="G24" s="8"/>
+      <c r="H24" s="8">
         <f t="shared" si="2"/>
         <v>0.000226076666666667</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I24" s="8">
         <f t="shared" si="2"/>
         <v>0.021983016</v>
       </c>
-      <c r="J24" s="10">
+      <c r="J24" s="8">
         <f t="shared" si="2"/>
         <v>26.7794600283333</v>
       </c>
-      <c r="K24" s="10">
+      <c r="K24" s="8">
         <f t="shared" si="2"/>
         <v>13.668895784</v>
       </c>
@@ -18041,689 +18036,689 @@
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="2:11">
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="13">
+      <c r="C28" s="11">
         <v>0.025055166</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28" s="11">
         <v>0.247933203</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="11">
         <v>0.003275336</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28" s="11">
         <v>0.096691252</v>
       </c>
-      <c r="G28" s="19"/>
-      <c r="H28" s="13">
+      <c r="G28" s="17"/>
+      <c r="H28" s="11">
         <v>0.000208207</v>
       </c>
-      <c r="I28" s="13">
+      <c r="I28" s="11">
         <v>0.025928089</v>
       </c>
-      <c r="J28" s="13">
+      <c r="J28" s="11">
         <v>0.246443876</v>
       </c>
-      <c r="K28" s="13">
+      <c r="K28" s="11">
         <v>0.150675694</v>
       </c>
     </row>
     <row r="29" spans="2:11">
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C29" s="11">
         <v>0.027369866</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="11">
         <v>0.163165832</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="11">
         <v>0.003308852</v>
       </c>
-      <c r="F29" s="13">
+      <c r="F29" s="11">
         <v>0.101819582</v>
       </c>
-      <c r="G29" s="19"/>
-      <c r="H29" s="13">
+      <c r="G29" s="17"/>
+      <c r="H29" s="11">
         <v>0.000218221</v>
       </c>
-      <c r="I29" s="13">
+      <c r="I29" s="11">
         <v>0.028954009</v>
       </c>
-      <c r="J29" s="13">
+      <c r="J29" s="11">
         <v>0.163392371</v>
       </c>
-      <c r="K29" s="13">
+      <c r="K29" s="11">
         <v>0.156498303</v>
       </c>
     </row>
     <row r="30" spans="2:11">
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="13">
+      <c r="C30" s="11">
         <v>0.025469956</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30" s="11">
         <v>0.56881678</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="11">
         <v>0.003286984</v>
       </c>
-      <c r="F30" s="13">
+      <c r="F30" s="11">
         <v>0.108363884</v>
       </c>
-      <c r="G30" s="19"/>
-      <c r="H30" s="13">
+      <c r="G30" s="17"/>
+      <c r="H30" s="11">
         <v>0.000221592</v>
       </c>
-      <c r="I30" s="13">
+      <c r="I30" s="11">
         <v>0.024968787</v>
       </c>
-      <c r="J30" s="13">
+      <c r="J30" s="11">
         <v>0.570690689</v>
       </c>
-      <c r="K30" s="13">
+      <c r="K30" s="11">
         <v>0.17546829</v>
       </c>
     </row>
     <row r="31" spans="2:11">
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="10">
         <f>AVERAGE(C28:C30)</f>
         <v>0.025964996</v>
       </c>
-      <c r="D31" s="12">
+      <c r="D31" s="10">
         <f t="shared" ref="D31:K31" si="3">AVERAGE(D28:D30)</f>
         <v>0.326638605</v>
       </c>
-      <c r="E31" s="12">
+      <c r="E31" s="10">
         <f t="shared" si="3"/>
         <v>0.00329039066666667</v>
       </c>
-      <c r="F31" s="12">
+      <c r="F31" s="10">
         <f t="shared" si="3"/>
         <v>0.102291572666667</v>
       </c>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12">
+      <c r="G31" s="10"/>
+      <c r="H31" s="10">
         <f t="shared" si="3"/>
         <v>0.000216006666666667</v>
       </c>
-      <c r="I31" s="12">
+      <c r="I31" s="10">
         <f t="shared" si="3"/>
         <v>0.0266169616666667</v>
       </c>
-      <c r="J31" s="12">
+      <c r="J31" s="10">
         <f t="shared" si="3"/>
         <v>0.326842312</v>
       </c>
-      <c r="K31" s="12">
+      <c r="K31" s="10">
         <f t="shared" si="3"/>
         <v>0.160880762333333</v>
       </c>
     </row>
     <row r="32" spans="2:11">
-      <c r="B32" s="14"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
     </row>
     <row r="33" spans="2:11">
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C33" s="11">
         <v>0.02618346</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D33" s="11">
         <v>0.593741083</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="11">
         <v>0.021560048</v>
       </c>
-      <c r="F33" s="13">
+      <c r="F33" s="11">
         <v>0.316747042</v>
       </c>
-      <c r="G33" s="19"/>
-      <c r="H33" s="13">
+      <c r="G33" s="17"/>
+      <c r="H33" s="11">
         <v>0.000217854</v>
       </c>
-      <c r="I33" s="13">
+      <c r="I33" s="11">
         <v>0.029427946</v>
       </c>
-      <c r="J33" s="13">
+      <c r="J33" s="11">
         <v>0.589607373</v>
       </c>
-      <c r="K33" s="13">
+      <c r="K33" s="11">
         <v>0.554321044</v>
       </c>
     </row>
     <row r="34" spans="2:11">
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C34" s="11">
         <v>0.022920588</v>
       </c>
-      <c r="D34" s="13">
+      <c r="D34" s="11">
         <v>0.62379908</v>
       </c>
-      <c r="E34" s="13">
+      <c r="E34" s="11">
         <v>0.026077227</v>
       </c>
-      <c r="F34" s="13">
+      <c r="F34" s="11">
         <v>0.286310457</v>
       </c>
-      <c r="G34" s="19"/>
-      <c r="H34" s="13">
+      <c r="G34" s="17"/>
+      <c r="H34" s="11">
         <v>0.000240865</v>
       </c>
-      <c r="I34" s="13">
+      <c r="I34" s="11">
         <v>0.022576184</v>
       </c>
-      <c r="J34" s="13">
+      <c r="J34" s="11">
         <v>0.623658317</v>
       </c>
-      <c r="K34" s="13">
+      <c r="K34" s="11">
         <v>0.450708624</v>
       </c>
     </row>
     <row r="35" spans="2:11">
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="13">
+      <c r="C35" s="11">
         <v>0.022397519</v>
       </c>
-      <c r="D35" s="13">
+      <c r="D35" s="11">
         <v>0.534016778</v>
       </c>
-      <c r="E35" s="13">
+      <c r="E35" s="11">
         <v>0.021913278</v>
       </c>
-      <c r="F35" s="13">
+      <c r="F35" s="11">
         <v>0.232526877</v>
       </c>
-      <c r="G35" s="19"/>
-      <c r="H35" s="13">
+      <c r="G35" s="17"/>
+      <c r="H35" s="11">
         <v>0.000214601</v>
       </c>
-      <c r="I35" s="13">
+      <c r="I35" s="11">
         <v>0.022466446</v>
       </c>
-      <c r="J35" s="13">
+      <c r="J35" s="11">
         <v>0.533248518</v>
       </c>
-      <c r="K35" s="13">
+      <c r="K35" s="11">
         <v>0.447878661</v>
       </c>
     </row>
     <row r="36" spans="2:11">
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="12">
+      <c r="C36" s="10">
         <f>AVERAGE(C33:C35)</f>
         <v>0.0238338556666667</v>
       </c>
-      <c r="D36" s="12">
+      <c r="D36" s="10">
         <f t="shared" ref="D36:K36" si="4">AVERAGE(D33:D35)</f>
         <v>0.583852313666667</v>
       </c>
-      <c r="E36" s="12">
+      <c r="E36" s="10">
         <f t="shared" si="4"/>
         <v>0.0231835176666667</v>
       </c>
-      <c r="F36" s="12">
+      <c r="F36" s="10">
         <f t="shared" si="4"/>
         <v>0.278528125333333</v>
       </c>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12">
+      <c r="G36" s="10"/>
+      <c r="H36" s="10">
         <f t="shared" si="4"/>
         <v>0.00022444</v>
       </c>
-      <c r="I36" s="12">
+      <c r="I36" s="10">
         <f t="shared" si="4"/>
         <v>0.0248235253333333</v>
       </c>
-      <c r="J36" s="12">
+      <c r="J36" s="10">
         <f t="shared" si="4"/>
         <v>0.582171402666667</v>
       </c>
-      <c r="K36" s="12">
+      <c r="K36" s="10">
         <f t="shared" si="4"/>
         <v>0.484302776333333</v>
       </c>
     </row>
     <row r="37" spans="2:11">
-      <c r="B37" s="14"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
     </row>
     <row r="38" spans="2:11">
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="13">
+      <c r="C38" s="11">
         <v>0.040202329</v>
       </c>
-      <c r="D38" s="13">
+      <c r="D38" s="11">
         <v>1.189469381</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E38" s="11">
         <v>0.136013268</v>
       </c>
-      <c r="F38" s="13">
+      <c r="F38" s="11">
         <v>0.933518279</v>
       </c>
-      <c r="G38" s="19"/>
-      <c r="H38" s="13">
+      <c r="G38" s="17"/>
+      <c r="H38" s="11">
         <v>0.000210498</v>
       </c>
-      <c r="I38" s="13">
+      <c r="I38" s="11">
         <v>0.025258014</v>
       </c>
-      <c r="J38" s="13">
+      <c r="J38" s="11">
         <v>1.187052442</v>
       </c>
-      <c r="K38" s="13">
+      <c r="K38" s="11">
         <v>1.600107903</v>
       </c>
     </row>
     <row r="39" spans="2:11">
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="13">
+      <c r="C39" s="11">
         <v>0.024531267</v>
       </c>
-      <c r="D39" s="13">
+      <c r="D39" s="11">
         <v>1.211228665</v>
       </c>
-      <c r="E39" s="13">
+      <c r="E39" s="11">
         <v>0.155723427</v>
       </c>
-      <c r="F39" s="13">
+      <c r="F39" s="11">
         <v>0.715251809</v>
       </c>
-      <c r="G39" s="19"/>
-      <c r="H39" s="13">
+      <c r="G39" s="17"/>
+      <c r="H39" s="11">
         <v>0.00020394</v>
       </c>
-      <c r="I39" s="13">
+      <c r="I39" s="11">
         <v>0.024134549</v>
       </c>
-      <c r="J39" s="13">
+      <c r="J39" s="11">
         <v>1.214362526</v>
       </c>
-      <c r="K39" s="13">
+      <c r="K39" s="11">
         <v>1.352519098</v>
       </c>
     </row>
     <row r="40" spans="2:11">
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="13">
+      <c r="C40" s="11">
         <v>0.02657904</v>
       </c>
-      <c r="D40" s="13">
+      <c r="D40" s="11">
         <v>1.157132962</v>
       </c>
-      <c r="E40" s="13">
+      <c r="E40" s="11">
         <v>0.134310907</v>
       </c>
-      <c r="F40" s="13">
+      <c r="F40" s="11">
         <v>0.773510768</v>
       </c>
-      <c r="G40" s="19"/>
-      <c r="H40" s="13">
+      <c r="G40" s="17"/>
+      <c r="H40" s="11">
         <v>0.000211912</v>
       </c>
-      <c r="I40" s="13">
+      <c r="I40" s="11">
         <v>0.026083245</v>
       </c>
-      <c r="J40" s="13">
+      <c r="J40" s="11">
         <v>1.156829879</v>
       </c>
-      <c r="K40" s="13">
+      <c r="K40" s="11">
         <v>1.36859325</v>
       </c>
     </row>
     <row r="41" spans="2:11">
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="12">
+      <c r="C41" s="10">
         <f>AVERAGE(C38:C40)</f>
         <v>0.0304375453333333</v>
       </c>
-      <c r="D41" s="12">
+      <c r="D41" s="10">
         <f t="shared" ref="D41:K41" si="5">AVERAGE(D38:D40)</f>
         <v>1.18594366933333</v>
       </c>
-      <c r="E41" s="12">
+      <c r="E41" s="10">
         <f t="shared" si="5"/>
         <v>0.142015867333333</v>
       </c>
-      <c r="F41" s="12">
+      <c r="F41" s="10">
         <f t="shared" si="5"/>
         <v>0.807426952</v>
       </c>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12">
+      <c r="G41" s="10"/>
+      <c r="H41" s="10">
         <f t="shared" si="5"/>
         <v>0.000208783333333333</v>
       </c>
-      <c r="I41" s="12">
+      <c r="I41" s="10">
         <f t="shared" si="5"/>
         <v>0.0251586026666667</v>
       </c>
-      <c r="J41" s="12">
+      <c r="J41" s="10">
         <f t="shared" si="5"/>
         <v>1.18608161566667</v>
       </c>
-      <c r="K41" s="12">
+      <c r="K41" s="10">
         <f t="shared" si="5"/>
         <v>1.44040675033333</v>
       </c>
     </row>
     <row r="42" spans="2:11">
-      <c r="B42" s="14"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
     </row>
     <row r="43" spans="2:11">
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C43" s="13">
+      <c r="C43" s="11">
         <v>0.022578778</v>
       </c>
-      <c r="D43" s="13">
+      <c r="D43" s="11">
         <v>7.083389961</v>
       </c>
-      <c r="E43" s="13">
+      <c r="E43" s="11">
         <v>1.519721135</v>
       </c>
-      <c r="F43" s="13">
+      <c r="F43" s="11">
         <v>4.024134693</v>
       </c>
-      <c r="G43" s="19"/>
-      <c r="H43" s="13">
+      <c r="G43" s="17"/>
+      <c r="H43" s="11">
         <v>0.000316662</v>
       </c>
-      <c r="I43" s="13">
+      <c r="I43" s="11">
         <v>0.022031625</v>
       </c>
-      <c r="J43" s="13">
+      <c r="J43" s="11">
         <v>7.085071565</v>
       </c>
-      <c r="K43" s="13">
+      <c r="K43" s="11">
         <v>6.626158613</v>
       </c>
     </row>
     <row r="44" spans="2:11">
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="13">
+      <c r="C44" s="11">
         <v>0.022415248</v>
       </c>
-      <c r="D44" s="13">
+      <c r="D44" s="11">
         <v>4.854897028</v>
       </c>
-      <c r="E44" s="13">
+      <c r="E44" s="11">
         <v>1.627724206</v>
       </c>
-      <c r="F44" s="13">
+      <c r="F44" s="11">
         <v>3.988542487</v>
       </c>
-      <c r="G44" s="19"/>
-      <c r="H44" s="13">
+      <c r="G44" s="17"/>
+      <c r="H44" s="11">
         <v>0.000206478</v>
       </c>
-      <c r="I44" s="13">
+      <c r="I44" s="11">
         <v>0.02235752</v>
       </c>
-      <c r="J44" s="13">
+      <c r="J44" s="11">
         <v>4.860848148</v>
       </c>
-      <c r="K44" s="13">
+      <c r="K44" s="11">
         <v>6.739035209</v>
       </c>
     </row>
     <row r="45" spans="2:11">
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C45" s="13">
+      <c r="C45" s="11">
         <v>0.023864747</v>
       </c>
-      <c r="D45" s="13">
+      <c r="D45" s="11">
         <v>4.710971304</v>
       </c>
-      <c r="E45" s="13">
+      <c r="E45" s="11">
         <v>1.625640027</v>
       </c>
-      <c r="F45" s="13">
+      <c r="F45" s="11">
         <v>3.982292571</v>
       </c>
-      <c r="G45" s="19"/>
-      <c r="H45" s="13">
+      <c r="G45" s="17"/>
+      <c r="H45" s="11">
         <v>0.000229689</v>
       </c>
-      <c r="I45" s="13">
+      <c r="I45" s="11">
         <v>0.024966431</v>
       </c>
-      <c r="J45" s="13">
+      <c r="J45" s="11">
         <v>4.826434975</v>
       </c>
-      <c r="K45" s="13">
+      <c r="K45" s="11">
         <v>6.473481438</v>
       </c>
     </row>
     <row r="46" spans="2:11">
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="12">
+      <c r="C46" s="10">
         <f>AVERAGE(C43:C45)</f>
         <v>0.0229529243333333</v>
       </c>
-      <c r="D46" s="12">
+      <c r="D46" s="10">
         <f t="shared" ref="D46:K46" si="6">AVERAGE(D43:D45)</f>
         <v>5.54975276433333</v>
       </c>
-      <c r="E46" s="12">
+      <c r="E46" s="10">
         <f t="shared" si="6"/>
         <v>1.591028456</v>
       </c>
-      <c r="F46" s="12">
+      <c r="F46" s="10">
         <f t="shared" si="6"/>
         <v>3.99832325033333</v>
       </c>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12">
+      <c r="G46" s="10"/>
+      <c r="H46" s="10">
         <f t="shared" si="6"/>
         <v>0.000250943</v>
       </c>
-      <c r="I46" s="12">
+      <c r="I46" s="10">
         <f t="shared" si="6"/>
         <v>0.0231185253333333</v>
       </c>
-      <c r="J46" s="12">
+      <c r="J46" s="10">
         <f t="shared" si="6"/>
         <v>5.590784896</v>
       </c>
-      <c r="K46" s="12">
+      <c r="K46" s="10">
         <f t="shared" si="6"/>
         <v>6.61289175333333</v>
       </c>
     </row>
     <row r="47" spans="2:11">
-      <c r="B47" s="14"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="13"/>
-      <c r="K47" s="13"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
     </row>
     <row r="48" spans="2:11">
-      <c r="B48" s="12" t="s">
+      <c r="B48" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C48" s="13">
+      <c r="C48" s="11">
         <v>0.022620046</v>
       </c>
-      <c r="D48" s="13">
+      <c r="D48" s="11">
         <v>23.25336059</v>
       </c>
-      <c r="E48" s="13">
+      <c r="E48" s="11">
         <v>12.360971954</v>
       </c>
-      <c r="F48" s="13">
+      <c r="F48" s="11">
         <v>21.512056645</v>
       </c>
-      <c r="G48" s="19"/>
-      <c r="H48" s="13">
+      <c r="G48" s="17"/>
+      <c r="H48" s="11">
         <v>0.000227924</v>
       </c>
-      <c r="I48" s="13">
+      <c r="I48" s="11">
         <v>0.022343414</v>
       </c>
-      <c r="J48" s="13">
+      <c r="J48" s="11">
         <v>23.252968495</v>
       </c>
-      <c r="K48" s="13">
+      <c r="K48" s="11">
         <v>37.521015941</v>
       </c>
     </row>
     <row r="49" spans="2:11">
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C49" s="13">
+      <c r="C49" s="11">
         <v>0.022936615</v>
       </c>
-      <c r="D49" s="13">
+      <c r="D49" s="11">
         <v>22.235235331</v>
       </c>
-      <c r="E49" s="13">
+      <c r="E49" s="11">
         <v>12.256516672</v>
       </c>
-      <c r="F49" s="13">
+      <c r="F49" s="11">
         <v>19.834867982</v>
       </c>
-      <c r="G49" s="19"/>
-      <c r="H49" s="13">
+      <c r="G49" s="17"/>
+      <c r="H49" s="11">
         <v>0.000210075</v>
       </c>
-      <c r="I49" s="13">
+      <c r="I49" s="11">
         <v>0.022686987</v>
       </c>
-      <c r="J49" s="13">
+      <c r="J49" s="11">
         <v>22.235804218</v>
       </c>
-      <c r="K49" s="13">
+      <c r="K49" s="11">
         <v>35.665064503</v>
       </c>
     </row>
     <row r="50" spans="2:11">
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C50" s="13">
+      <c r="C50" s="11">
         <v>0.025266154</v>
       </c>
-      <c r="D50" s="13">
+      <c r="D50" s="11">
         <v>19.11133263</v>
       </c>
-      <c r="E50" s="13">
+      <c r="E50" s="11">
         <v>12.350615764</v>
       </c>
-      <c r="F50" s="13">
+      <c r="F50" s="11">
         <v>22.83088109</v>
       </c>
-      <c r="G50" s="19"/>
-      <c r="H50" s="13">
+      <c r="G50" s="17"/>
+      <c r="H50" s="11">
         <v>0.000208478</v>
       </c>
-      <c r="I50" s="13">
+      <c r="I50" s="11">
         <v>0.024735756</v>
       </c>
-      <c r="J50" s="13">
+      <c r="J50" s="11">
         <v>19.11078268</v>
       </c>
-      <c r="K50" s="13">
+      <c r="K50" s="11">
         <v>38.722622304</v>
       </c>
     </row>
     <row r="51" spans="2:11">
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C51" s="12">
+      <c r="C51" s="10">
         <f>AVERAGE(C48:C50)</f>
         <v>0.023607605</v>
       </c>
-      <c r="D51" s="12">
+      <c r="D51" s="10">
         <f t="shared" ref="D51:K51" si="7">AVERAGE(D48:D50)</f>
         <v>21.533309517</v>
       </c>
-      <c r="E51" s="12">
+      <c r="E51" s="10">
         <f t="shared" si="7"/>
         <v>12.3227014633333</v>
       </c>
-      <c r="F51" s="12">
+      <c r="F51" s="10">
         <f t="shared" si="7"/>
         <v>21.3926019056667</v>
       </c>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12">
+      <c r="G51" s="10"/>
+      <c r="H51" s="10">
         <f t="shared" si="7"/>
         <v>0.000215492333333333</v>
       </c>
-      <c r="I51" s="12">
+      <c r="I51" s="10">
         <f t="shared" si="7"/>
         <v>0.0232553856666667</v>
       </c>
-      <c r="J51" s="12">
+      <c r="J51" s="10">
         <f t="shared" si="7"/>
         <v>21.533185131</v>
       </c>
-      <c r="K51" s="12">
+      <c r="K51" s="10">
         <f t="shared" si="7"/>
         <v>37.302900916</v>
       </c>
@@ -18742,829 +18737,829 @@
       <c r="G54" s="1"/>
     </row>
     <row r="56" spans="2:11">
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C56" s="11">
+      <c r="C56" s="9">
         <v>0.00073095</v>
       </c>
-      <c r="D56" s="11">
+      <c r="D56" s="9">
         <v>0.031289033</v>
       </c>
-      <c r="E56" s="11">
+      <c r="E56" s="9">
         <v>0.006908466</v>
       </c>
-      <c r="F56" s="11">
+      <c r="F56" s="9">
         <v>0.030913232</v>
       </c>
-      <c r="G56" s="17"/>
-      <c r="H56" s="11">
+      <c r="G56" s="15"/>
+      <c r="H56" s="9">
         <v>0.000199435</v>
       </c>
-      <c r="I56" s="11">
+      <c r="I56" s="9">
         <v>0.000457031</v>
       </c>
-      <c r="J56" s="11">
+      <c r="J56" s="9">
         <v>0.031279328</v>
       </c>
-      <c r="K56" s="11">
+      <c r="K56" s="9">
         <v>0.049038855</v>
       </c>
     </row>
     <row r="57" spans="2:11">
-      <c r="B57" s="15" t="s">
+      <c r="B57" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="11">
+      <c r="C57" s="9">
         <v>0.00070261</v>
       </c>
-      <c r="D57" s="11">
+      <c r="D57" s="9">
         <v>0.029077352</v>
       </c>
-      <c r="E57" s="11">
+      <c r="E57" s="9">
         <v>0.006468398</v>
       </c>
-      <c r="F57" s="11">
+      <c r="F57" s="9">
         <v>0.030576301</v>
       </c>
-      <c r="G57" s="17"/>
-      <c r="H57" s="11">
+      <c r="G57" s="15"/>
+      <c r="H57" s="9">
         <v>0.000217799</v>
       </c>
-      <c r="I57" s="11">
+      <c r="I57" s="9">
         <v>0.000288473</v>
       </c>
-      <c r="J57" s="11">
+      <c r="J57" s="9">
         <v>0.029116548</v>
       </c>
-      <c r="K57" s="11">
+      <c r="K57" s="9">
         <v>0.047800786</v>
       </c>
     </row>
     <row r="58" spans="2:11">
-      <c r="B58" s="15" t="s">
+      <c r="B58" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C58" s="11">
+      <c r="C58" s="9">
         <v>0.000714815</v>
       </c>
-      <c r="D58" s="11">
+      <c r="D58" s="9">
         <v>0.029588053</v>
       </c>
-      <c r="E58" s="11">
+      <c r="E58" s="9">
         <v>0.008639096</v>
       </c>
-      <c r="F58" s="11">
+      <c r="F58" s="9">
         <v>0.029809862</v>
       </c>
-      <c r="G58" s="17"/>
-      <c r="H58" s="11">
+      <c r="G58" s="15"/>
+      <c r="H58" s="9">
         <v>0.000200978</v>
       </c>
-      <c r="I58" s="11">
+      <c r="I58" s="9">
         <v>0.000346079</v>
       </c>
-      <c r="J58" s="11">
+      <c r="J58" s="9">
         <v>0.029679059</v>
       </c>
-      <c r="K58" s="11">
+      <c r="K58" s="9">
         <v>0.049140231</v>
       </c>
     </row>
     <row r="59" spans="2:11">
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C59" s="15">
+      <c r="C59" s="13">
         <f>AVERAGE(C56:C58)</f>
         <v>0.000716125</v>
       </c>
-      <c r="D59" s="15">
+      <c r="D59" s="13">
         <f t="shared" ref="D59:K59" si="8">AVERAGE(D56:D58)</f>
         <v>0.0299848126666667</v>
       </c>
-      <c r="E59" s="15">
+      <c r="E59" s="13">
         <f t="shared" si="8"/>
         <v>0.00733865333333333</v>
       </c>
-      <c r="F59" s="15">
+      <c r="F59" s="13">
         <f t="shared" si="8"/>
         <v>0.0304331316666667</v>
       </c>
-      <c r="G59" s="15"/>
-      <c r="H59" s="15">
+      <c r="G59" s="13"/>
+      <c r="H59" s="13">
         <f t="shared" si="8"/>
         <v>0.000206070666666667</v>
       </c>
-      <c r="I59" s="15">
+      <c r="I59" s="13">
         <f t="shared" si="8"/>
         <v>0.000363861</v>
       </c>
-      <c r="J59" s="15">
+      <c r="J59" s="13">
         <f t="shared" si="8"/>
         <v>0.0300249783333333</v>
       </c>
-      <c r="K59" s="15">
+      <c r="K59" s="13">
         <f t="shared" si="8"/>
         <v>0.0486599573333333</v>
       </c>
     </row>
     <row r="60" spans="2:11">
-      <c r="B60" s="16"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="11"/>
-      <c r="K60" s="11"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
     </row>
     <row r="61" spans="2:11">
-      <c r="B61" s="15" t="s">
+      <c r="B61" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C61" s="11">
+      <c r="C61" s="9">
         <v>0.000765643</v>
       </c>
-      <c r="D61" s="11">
+      <c r="D61" s="9">
         <v>0.109876854</v>
       </c>
-      <c r="E61" s="11">
+      <c r="E61" s="9">
         <v>0.040157744</v>
       </c>
-      <c r="F61" s="11">
+      <c r="F61" s="9">
         <v>0.128090724</v>
       </c>
-      <c r="G61" s="17"/>
-      <c r="H61" s="11">
+      <c r="G61" s="15"/>
+      <c r="H61" s="9">
         <v>0.000303952</v>
       </c>
-      <c r="I61" s="11">
+      <c r="I61" s="9">
         <v>0.000345683</v>
       </c>
-      <c r="J61" s="11">
+      <c r="J61" s="9">
         <v>0.110164203</v>
       </c>
-      <c r="K61" s="11">
+      <c r="K61" s="9">
         <v>0.212318551</v>
       </c>
     </row>
     <row r="62" spans="2:11">
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C62" s="11">
+      <c r="C62" s="9">
         <v>0.000653564</v>
       </c>
-      <c r="D62" s="11">
+      <c r="D62" s="9">
         <v>0.112699486</v>
       </c>
-      <c r="E62" s="11">
+      <c r="E62" s="9">
         <v>0.040771423</v>
       </c>
-      <c r="F62" s="11">
+      <c r="F62" s="9">
         <v>0.127864484</v>
       </c>
-      <c r="G62" s="17"/>
-      <c r="H62" s="11">
+      <c r="G62" s="15"/>
+      <c r="H62" s="9">
         <v>0.000229317</v>
       </c>
-      <c r="I62" s="11">
+      <c r="I62" s="9">
         <v>0.000247059</v>
       </c>
-      <c r="J62" s="11">
+      <c r="J62" s="9">
         <v>0.11280743</v>
       </c>
-      <c r="K62" s="11">
+      <c r="K62" s="9">
         <v>0.21100932</v>
       </c>
     </row>
     <row r="63" spans="2:11">
-      <c r="B63" s="15" t="s">
+      <c r="B63" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C63" s="11">
+      <c r="C63" s="9">
         <v>0.000675508</v>
       </c>
-      <c r="D63" s="11">
+      <c r="D63" s="9">
         <v>0.111434595</v>
       </c>
-      <c r="E63" s="11">
+      <c r="E63" s="9">
         <v>0.0366702</v>
       </c>
-      <c r="F63" s="11">
+      <c r="F63" s="9">
         <v>0.127719014</v>
       </c>
-      <c r="G63" s="17"/>
-      <c r="H63" s="11">
+      <c r="G63" s="15"/>
+      <c r="H63" s="9">
         <v>0.000295259</v>
       </c>
-      <c r="I63" s="11">
+      <c r="I63" s="9">
         <v>0.00024335</v>
       </c>
-      <c r="J63" s="11">
+      <c r="J63" s="9">
         <v>0.111544614</v>
       </c>
-      <c r="K63" s="11">
+      <c r="K63" s="9">
         <v>0.207503203</v>
       </c>
     </row>
     <row r="64" spans="2:11">
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C64" s="15">
+      <c r="C64" s="13">
         <f>AVERAGE(C61:C63)</f>
         <v>0.000698238333333333</v>
       </c>
-      <c r="D64" s="15">
+      <c r="D64" s="13">
         <f t="shared" ref="D64:K64" si="9">AVERAGE(D61:D63)</f>
         <v>0.111336978333333</v>
       </c>
-      <c r="E64" s="15">
+      <c r="E64" s="13">
         <f t="shared" si="9"/>
         <v>0.039199789</v>
       </c>
-      <c r="F64" s="15">
+      <c r="F64" s="13">
         <f t="shared" si="9"/>
         <v>0.127891407333333</v>
       </c>
-      <c r="G64" s="15"/>
-      <c r="H64" s="15">
+      <c r="G64" s="13"/>
+      <c r="H64" s="13">
         <f t="shared" si="9"/>
         <v>0.000276176</v>
       </c>
-      <c r="I64" s="15">
+      <c r="I64" s="13">
         <f t="shared" si="9"/>
         <v>0.000278697333333333</v>
       </c>
-      <c r="J64" s="15">
+      <c r="J64" s="13">
         <f t="shared" si="9"/>
         <v>0.111505415666667</v>
       </c>
-      <c r="K64" s="15">
+      <c r="K64" s="13">
         <f t="shared" si="9"/>
         <v>0.210277024666667</v>
       </c>
     </row>
     <row r="65" spans="2:11">
-      <c r="B65" s="16"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="17"/>
-      <c r="H65" s="11"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="11"/>
-      <c r="K65" s="11"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="9"/>
     </row>
     <row r="66" spans="2:11">
-      <c r="B66" s="15" t="s">
+      <c r="B66" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C66" s="11">
+      <c r="C66" s="9">
         <v>0.000767375</v>
       </c>
-      <c r="D66" s="11">
+      <c r="D66" s="9">
         <v>0.457059098</v>
       </c>
-      <c r="E66" s="11">
+      <c r="E66" s="9">
         <v>0.24952992</v>
       </c>
-      <c r="F66" s="11">
+      <c r="F66" s="9">
         <v>0.352701954</v>
       </c>
-      <c r="G66" s="17"/>
-      <c r="H66" s="11">
+      <c r="G66" s="15"/>
+      <c r="H66" s="9">
         <v>0.000215648</v>
       </c>
-      <c r="I66" s="11">
+      <c r="I66" s="9">
         <v>0.000402061</v>
       </c>
-      <c r="J66" s="11">
+      <c r="J66" s="9">
         <v>0.457101295</v>
       </c>
-      <c r="K66" s="11">
+      <c r="K66" s="9">
         <v>0.781997394</v>
       </c>
     </row>
     <row r="67" spans="2:11">
-      <c r="B67" s="15" t="s">
+      <c r="B67" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C67" s="11">
+      <c r="C67" s="9">
         <v>0.000702049</v>
       </c>
-      <c r="D67" s="11">
+      <c r="D67" s="9">
         <v>0.452455178</v>
       </c>
-      <c r="E67" s="11">
+      <c r="E67" s="9">
         <v>0.250086256</v>
       </c>
-      <c r="F67" s="11">
+      <c r="F67" s="9">
         <v>0.35541828</v>
       </c>
-      <c r="G67" s="17"/>
-      <c r="H67" s="11">
+      <c r="G67" s="15"/>
+      <c r="H67" s="9">
         <v>0.000209451</v>
       </c>
-      <c r="I67" s="11">
+      <c r="I67" s="9">
         <v>0.000305484</v>
       </c>
-      <c r="J67" s="11">
+      <c r="J67" s="9">
         <v>0.452547765</v>
       </c>
-      <c r="K67" s="11">
+      <c r="K67" s="9">
         <v>0.780998495</v>
       </c>
     </row>
     <row r="68" spans="2:11">
-      <c r="B68" s="15" t="s">
+      <c r="B68" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C68" s="11">
+      <c r="C68" s="9">
         <v>0.000654664</v>
       </c>
-      <c r="D68" s="11">
+      <c r="D68" s="9">
         <v>0.457711239</v>
       </c>
-      <c r="E68" s="11">
+      <c r="E68" s="9">
         <v>0.248394666</v>
       </c>
-      <c r="F68" s="11">
+      <c r="F68" s="9">
         <v>0.347573768</v>
       </c>
-      <c r="G68" s="17"/>
-      <c r="H68" s="11">
+      <c r="G68" s="15"/>
+      <c r="H68" s="9">
         <v>0.00019136</v>
       </c>
-      <c r="I68" s="11">
+      <c r="I68" s="9">
         <v>0.000263651</v>
       </c>
-      <c r="J68" s="11">
+      <c r="J68" s="9">
         <v>0.457824693</v>
       </c>
-      <c r="K68" s="11">
+      <c r="K68" s="9">
         <v>0.773464733</v>
       </c>
     </row>
     <row r="69" spans="2:11">
-      <c r="B69" s="15" t="s">
+      <c r="B69" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C69" s="15">
+      <c r="C69" s="13">
         <f>AVERAGE(C66:C68)</f>
         <v>0.000708029333333333</v>
       </c>
-      <c r="D69" s="15">
+      <c r="D69" s="13">
         <f t="shared" ref="D69:K69" si="10">AVERAGE(D66:D68)</f>
         <v>0.455741838333333</v>
       </c>
-      <c r="E69" s="15">
+      <c r="E69" s="13">
         <f t="shared" si="10"/>
         <v>0.249336947333333</v>
       </c>
-      <c r="F69" s="15">
+      <c r="F69" s="13">
         <f t="shared" si="10"/>
         <v>0.351898000666667</v>
       </c>
-      <c r="G69" s="15"/>
-      <c r="H69" s="15">
+      <c r="G69" s="13"/>
+      <c r="H69" s="13">
         <f t="shared" si="10"/>
         <v>0.000205486333333333</v>
       </c>
-      <c r="I69" s="15">
+      <c r="I69" s="13">
         <f t="shared" si="10"/>
         <v>0.000323732</v>
       </c>
-      <c r="J69" s="15">
+      <c r="J69" s="13">
         <f t="shared" si="10"/>
         <v>0.455824584333333</v>
       </c>
-      <c r="K69" s="15">
+      <c r="K69" s="13">
         <f t="shared" si="10"/>
         <v>0.778820207333333</v>
       </c>
     </row>
     <row r="70" spans="2:11">
-      <c r="B70" s="16"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
-      <c r="G70" s="17"/>
-      <c r="H70" s="11"/>
-      <c r="I70" s="11"/>
-      <c r="J70" s="11"/>
-      <c r="K70" s="11"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="9"/>
+      <c r="J70" s="9"/>
+      <c r="K70" s="9"/>
     </row>
     <row r="71" spans="2:11">
-      <c r="B71" s="15" t="s">
+      <c r="B71" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C71" s="11">
+      <c r="C71" s="9">
         <v>0.000825866</v>
       </c>
-      <c r="D71" s="11">
+      <c r="D71" s="9">
         <v>1.907514152</v>
       </c>
-      <c r="E71" s="11">
+      <c r="E71" s="9">
         <v>1.907259393</v>
       </c>
-      <c r="F71" s="11">
+      <c r="F71" s="9">
         <v>1.325549354</v>
       </c>
-      <c r="G71" s="17"/>
-      <c r="H71" s="11">
+      <c r="G71" s="15"/>
+      <c r="H71" s="9">
         <v>0.000222991</v>
       </c>
-      <c r="I71" s="11">
+      <c r="I71" s="9">
         <v>0.000307106</v>
       </c>
-      <c r="J71" s="11">
+      <c r="J71" s="9">
         <v>1.907713951</v>
       </c>
-      <c r="K71" s="11">
+      <c r="K71" s="9">
         <v>4.008240167</v>
       </c>
     </row>
     <row r="72" spans="2:11">
-      <c r="B72" s="15" t="s">
+      <c r="B72" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C72" s="11">
+      <c r="C72" s="9">
         <v>0.000828967</v>
       </c>
-      <c r="D72" s="11">
+      <c r="D72" s="9">
         <v>1.889865961</v>
       </c>
-      <c r="E72" s="11">
+      <c r="E72" s="9">
         <v>1.908989792</v>
       </c>
-      <c r="F72" s="11">
+      <c r="F72" s="9">
         <v>1.319447915</v>
       </c>
-      <c r="G72" s="17"/>
-      <c r="H72" s="11">
+      <c r="G72" s="15"/>
+      <c r="H72" s="9">
         <v>0.000195436</v>
       </c>
-      <c r="I72" s="11">
+      <c r="I72" s="9">
         <v>0.000577182</v>
       </c>
-      <c r="J72" s="11">
+      <c r="J72" s="9">
         <v>1.889880758</v>
       </c>
-      <c r="K72" s="11">
+      <c r="K72" s="9">
         <v>3.990396526</v>
       </c>
     </row>
     <row r="73" spans="2:11">
-      <c r="B73" s="15" t="s">
+      <c r="B73" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C73" s="11">
+      <c r="C73" s="9">
         <v>0.000703103</v>
       </c>
-      <c r="D73" s="11">
+      <c r="D73" s="9">
         <v>1.895198315</v>
       </c>
-      <c r="E73" s="11">
+      <c r="E73" s="9">
         <v>1.902380342</v>
       </c>
-      <c r="F73" s="11">
+      <c r="F73" s="9">
         <v>1.315671753</v>
       </c>
-      <c r="G73" s="17"/>
-      <c r="H73" s="11">
+      <c r="G73" s="15"/>
+      <c r="H73" s="9">
         <v>0.000206638</v>
       </c>
-      <c r="I73" s="11">
+      <c r="I73" s="9">
         <v>0.000350356</v>
       </c>
-      <c r="J73" s="11">
+      <c r="J73" s="9">
         <v>1.89527455</v>
       </c>
-      <c r="K73" s="11">
+      <c r="K73" s="9">
         <v>3.982449722</v>
       </c>
     </row>
     <row r="74" spans="2:11">
-      <c r="B74" s="15" t="s">
+      <c r="B74" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C74" s="15">
+      <c r="C74" s="13">
         <f>AVERAGE(C71:C73)</f>
         <v>0.000785978666666667</v>
       </c>
-      <c r="D74" s="15">
+      <c r="D74" s="13">
         <f t="shared" ref="D74:K74" si="11">AVERAGE(D71:D73)</f>
         <v>1.89752614266667</v>
       </c>
-      <c r="E74" s="15">
+      <c r="E74" s="13">
         <f t="shared" si="11"/>
         <v>1.90620984233333</v>
       </c>
-      <c r="F74" s="15">
+      <c r="F74" s="13">
         <f t="shared" si="11"/>
         <v>1.32022300733333</v>
       </c>
-      <c r="G74" s="15"/>
-      <c r="H74" s="15">
+      <c r="G74" s="13"/>
+      <c r="H74" s="13">
         <f t="shared" si="11"/>
         <v>0.000208355</v>
       </c>
-      <c r="I74" s="15">
+      <c r="I74" s="13">
         <f t="shared" si="11"/>
         <v>0.000411548</v>
       </c>
-      <c r="J74" s="15">
+      <c r="J74" s="13">
         <f t="shared" si="11"/>
         <v>1.89762308633333</v>
       </c>
-      <c r="K74" s="15">
+      <c r="K74" s="13">
         <f t="shared" si="11"/>
         <v>3.99369547166667</v>
       </c>
     </row>
     <row r="75" spans="2:11">
-      <c r="B75" s="16"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11"/>
-      <c r="E75" s="11"/>
-      <c r="F75" s="11"/>
-      <c r="G75" s="17"/>
-      <c r="H75" s="11"/>
-      <c r="I75" s="11"/>
-      <c r="J75" s="11"/>
-      <c r="K75" s="11"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="9"/>
+      <c r="J75" s="9"/>
+      <c r="K75" s="9"/>
     </row>
     <row r="76" spans="2:11">
-      <c r="B76" s="15" t="s">
+      <c r="B76" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C76" s="11">
+      <c r="C76" s="9">
         <v>0.000770064</v>
       </c>
-      <c r="D76" s="11">
+      <c r="D76" s="9">
         <v>8.075835083</v>
       </c>
-      <c r="E76" s="11">
+      <c r="E76" s="9">
         <v>14.945429906</v>
       </c>
-      <c r="F76" s="11">
+      <c r="F76" s="9">
         <v>5.27623465</v>
       </c>
-      <c r="G76" s="17"/>
-      <c r="H76" s="11">
+      <c r="G76" s="15"/>
+      <c r="H76" s="9">
         <v>0.000194628</v>
       </c>
-      <c r="I76" s="11">
+      <c r="I76" s="9">
         <v>0.000444901</v>
       </c>
-      <c r="J76" s="11">
+      <c r="J76" s="9">
         <v>8.075929746</v>
       </c>
-      <c r="K76" s="11">
+      <c r="K76" s="9">
         <v>23.603262922</v>
       </c>
     </row>
     <row r="77" spans="2:11">
-      <c r="B77" s="15" t="s">
+      <c r="B77" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C77" s="11">
+      <c r="C77" s="9">
         <v>0.000726632</v>
       </c>
-      <c r="D77" s="11">
+      <c r="D77" s="9">
         <v>7.947250902</v>
       </c>
-      <c r="E77" s="11">
+      <c r="E77" s="9">
         <v>14.935579324</v>
       </c>
-      <c r="F77" s="11">
+      <c r="F77" s="9">
         <v>5.272265761</v>
       </c>
-      <c r="G77" s="17"/>
-      <c r="H77" s="11">
+      <c r="G77" s="15"/>
+      <c r="H77" s="9">
         <v>0.000250759</v>
       </c>
-      <c r="I77" s="11">
+      <c r="I77" s="9">
         <v>0.000353042</v>
       </c>
-      <c r="J77" s="11">
+      <c r="J77" s="9">
         <v>7.947315043</v>
       </c>
-      <c r="K77" s="11">
+      <c r="K77" s="9">
         <v>23.526334308</v>
       </c>
     </row>
     <row r="78" spans="2:11">
-      <c r="B78" s="15" t="s">
+      <c r="B78" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C78" s="11">
+      <c r="C78" s="9">
         <v>0.000671476</v>
       </c>
-      <c r="D78" s="11">
+      <c r="D78" s="9">
         <v>7.954970245</v>
       </c>
-      <c r="E78" s="11">
+      <c r="E78" s="9">
         <v>14.961849949</v>
       </c>
-      <c r="F78" s="11">
+      <c r="F78" s="9">
         <v>5.272723511</v>
       </c>
-      <c r="G78" s="17"/>
-      <c r="H78" s="11">
+      <c r="G78" s="15"/>
+      <c r="H78" s="9">
         <v>0.0001955</v>
       </c>
-      <c r="I78" s="11">
+      <c r="I78" s="9">
         <v>0.000259074</v>
       </c>
-      <c r="J78" s="11">
+      <c r="J78" s="9">
         <v>7.955064078</v>
       </c>
-      <c r="K78" s="11">
+      <c r="K78" s="9">
         <v>23.550159942</v>
       </c>
     </row>
     <row r="79" spans="2:11">
-      <c r="B79" s="15" t="s">
+      <c r="B79" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C79" s="15">
+      <c r="C79" s="13">
         <f>AVERAGE(C76:C78)</f>
         <v>0.000722724</v>
       </c>
-      <c r="D79" s="15">
+      <c r="D79" s="13">
         <f t="shared" ref="D79:K79" si="12">AVERAGE(D76:D78)</f>
         <v>7.99268541</v>
       </c>
-      <c r="E79" s="15">
+      <c r="E79" s="13">
         <f t="shared" si="12"/>
         <v>14.9476197263333</v>
       </c>
-      <c r="F79" s="15">
+      <c r="F79" s="13">
         <f t="shared" si="12"/>
         <v>5.27374130733333</v>
       </c>
-      <c r="G79" s="15"/>
-      <c r="H79" s="15">
+      <c r="G79" s="13"/>
+      <c r="H79" s="13">
         <f t="shared" si="12"/>
         <v>0.000213629</v>
       </c>
-      <c r="I79" s="15">
+      <c r="I79" s="13">
         <f t="shared" si="12"/>
         <v>0.000352339</v>
       </c>
-      <c r="J79" s="15">
+      <c r="J79" s="13">
         <f t="shared" si="12"/>
         <v>7.99276962233333</v>
       </c>
-      <c r="K79" s="15">
+      <c r="K79" s="13">
         <f t="shared" si="12"/>
         <v>23.5599190573333</v>
       </c>
     </row>
     <row r="80" spans="2:11">
-      <c r="B80" s="16"/>
-      <c r="C80" s="11"/>
-      <c r="D80" s="11"/>
-      <c r="E80" s="11"/>
-      <c r="F80" s="11"/>
-      <c r="G80" s="17"/>
-      <c r="H80" s="11"/>
-      <c r="I80" s="11"/>
-      <c r="J80" s="11"/>
-      <c r="K80" s="11"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="15"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="9"/>
+      <c r="J80" s="9"/>
+      <c r="K80" s="9"/>
     </row>
     <row r="81" spans="2:11">
-      <c r="B81" s="15" t="s">
+      <c r="B81" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C81" s="11">
+      <c r="C81" s="9">
         <v>0.000626324</v>
       </c>
-      <c r="D81" s="11">
+      <c r="D81" s="9">
         <v>33.447083914</v>
       </c>
-      <c r="E81" s="11">
+      <c r="E81" s="9">
         <v>118.393712856</v>
       </c>
-      <c r="F81" s="11">
+      <c r="F81" s="9">
         <v>20.865503994</v>
       </c>
-      <c r="G81" s="17"/>
-      <c r="H81" s="11">
+      <c r="G81" s="15"/>
+      <c r="H81" s="9">
         <v>0.000196488</v>
       </c>
-      <c r="I81" s="11">
+      <c r="I81" s="9">
         <v>0.000234789</v>
       </c>
-      <c r="J81" s="11">
+      <c r="J81" s="9">
         <v>33.448433821</v>
       </c>
-      <c r="K81" s="11">
+      <c r="K81" s="9">
         <v>153.275475035</v>
       </c>
     </row>
     <row r="82" spans="2:11">
-      <c r="B82" s="15" t="s">
+      <c r="B82" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C82" s="11">
+      <c r="C82" s="9">
         <v>0.00066923</v>
       </c>
-      <c r="D82" s="11">
+      <c r="D82" s="9">
         <v>32.960691102</v>
       </c>
-      <c r="E82" s="11">
+      <c r="E82" s="9">
         <v>118.280934997</v>
       </c>
-      <c r="F82" s="11">
+      <c r="F82" s="9">
         <v>20.647518216</v>
       </c>
-      <c r="G82" s="17"/>
-      <c r="H82" s="11">
+      <c r="G82" s="15"/>
+      <c r="H82" s="9">
         <v>0.000196291</v>
       </c>
-      <c r="I82" s="11">
+      <c r="I82" s="9">
         <v>0.000301484</v>
       </c>
-      <c r="J82" s="11">
+      <c r="J82" s="9">
         <v>32.961410494</v>
       </c>
-      <c r="K82" s="11">
+      <c r="K82" s="9">
         <v>152.691329016</v>
       </c>
     </row>
     <row r="83" spans="2:11">
-      <c r="B83" s="15" t="s">
+      <c r="B83" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C83" s="11">
+      <c r="C83" s="9">
         <v>0.000716528</v>
       </c>
-      <c r="D83" s="11">
+      <c r="D83" s="9">
         <v>33.104549791</v>
       </c>
-      <c r="E83" s="11">
+      <c r="E83" s="9">
         <v>118.385146584</v>
       </c>
-      <c r="F83" s="11">
+      <c r="F83" s="9">
         <v>20.709515861</v>
       </c>
-      <c r="G83" s="17"/>
-      <c r="H83" s="11">
+      <c r="G83" s="15"/>
+      <c r="H83" s="9">
         <v>0.000204811</v>
       </c>
-      <c r="I83" s="11">
+      <c r="I83" s="9">
         <v>0.000389881</v>
       </c>
-      <c r="J83" s="11">
+      <c r="J83" s="9">
         <v>33.10466388</v>
       </c>
-      <c r="K83" s="11">
+      <c r="K83" s="9">
         <v>152.89732083</v>
       </c>
     </row>
     <row r="84" spans="2:11">
-      <c r="B84" s="15" t="s">
+      <c r="B84" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C84" s="15">
+      <c r="C84" s="13">
         <f>AVERAGE(C81:C83)</f>
         <v>0.000670694</v>
       </c>
-      <c r="D84" s="15">
+      <c r="D84" s="13">
         <f t="shared" ref="D84:K84" si="13">AVERAGE(D81:D83)</f>
         <v>33.1707749356667</v>
       </c>
-      <c r="E84" s="15">
+      <c r="E84" s="13">
         <f t="shared" si="13"/>
         <v>118.353264812333</v>
       </c>
-      <c r="F84" s="15">
+      <c r="F84" s="13">
         <f t="shared" si="13"/>
         <v>20.7408460236667</v>
       </c>
-      <c r="G84" s="15"/>
-      <c r="H84" s="15">
+      <c r="G84" s="13"/>
+      <c r="H84" s="13">
         <f t="shared" si="13"/>
         <v>0.000199196666666667</v>
       </c>
-      <c r="I84" s="15">
+      <c r="I84" s="13">
         <f t="shared" si="13"/>
         <v>0.000308718</v>
       </c>
-      <c r="J84" s="15">
+      <c r="J84" s="13">
         <f t="shared" si="13"/>
         <v>33.1715027316667</v>
       </c>
-      <c r="K84" s="15">
+      <c r="K84" s="13">
         <f t="shared" si="13"/>
         <v>152.954708293667</v>
       </c>
@@ -19629,29 +19624,29 @@
       <c r="K3" s="1"/>
     </row>
     <row r="5" ht="28" customHeight="true" spans="3:11">
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -21178,15 +21173,15 @@
       <c r="E5" s="1">
         <v>29.21</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="2">
         <f>SUM(C5:E5)/3</f>
         <v>29.5166666666667</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="2">
         <f>F5-F5</f>
         <v>0</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="2">
         <v>0</v>
       </c>
     </row>
@@ -21203,15 +21198,15 @@
       <c r="E6" s="1">
         <v>21.44</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="2">
         <f>SUM(C6:E6)/3</f>
         <v>21.3033333333333</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="2">
         <f>F5-F6</f>
         <v>8.21333333333334</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="2">
         <f>((F5-F6)/F5)*100</f>
         <v>27.8260869565218</v>
       </c>
@@ -21229,15 +21224,15 @@
       <c r="E7" s="1">
         <v>18.25</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="2">
         <f>SUM(C7:E7)/3</f>
         <v>18.3833333333333</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="2">
         <f>F5-F7</f>
         <v>11.1333333333333</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="2">
         <f>((F5-F7)/F5)*100</f>
         <v>37.7188029361942</v>
       </c>
@@ -21255,15 +21250,15 @@
       <c r="E8" s="1">
         <v>17.34</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="2">
         <f>SUM(C8:E8)/3</f>
         <v>17.2733333333333</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="2">
         <f>F5-F8</f>
         <v>12.2433333333333</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="2">
         <f>((F5-F8)/F5)*100</f>
         <v>41.4793901750423</v>
       </c>
@@ -21281,15 +21276,15 @@
       <c r="E9" s="1">
         <v>17.41</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="2">
         <f>SUM(C9:E9)/3</f>
         <v>17.3766666666667</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="2">
         <f>F5-F9</f>
         <v>12.14</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="2">
         <f>((F5-F9)/F5)*100</f>
         <v>41.1293054771316</v>
       </c>
@@ -21337,15 +21332,15 @@
       <c r="E15" s="1">
         <v>51.65</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="2">
         <f t="shared" ref="F15:F19" si="0">SUM(C15:E15)/3</f>
         <v>51.8</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="2">
         <f>F15-F15</f>
         <v>0</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="2">
         <v>0</v>
       </c>
     </row>
@@ -21362,15 +21357,15 @@
       <c r="E16" s="1">
         <v>32.66</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="2">
         <f t="shared" si="0"/>
         <v>33.19</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="2">
         <f>F15-F16</f>
         <v>18.61</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="2">
         <f>((F15-F16)/F15)*100</f>
         <v>35.9266409266409</v>
       </c>
@@ -21388,15 +21383,15 @@
       <c r="E17" s="1">
         <v>27.88</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="2">
         <f t="shared" si="0"/>
         <v>27.5366666666667</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="2">
         <f>F15-F17</f>
         <v>24.2633333333333</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="2">
         <f>((F15-F17)/F15)*100</f>
         <v>46.8404118404118</v>
       </c>
@@ -21414,15 +21409,15 @@
       <c r="E18" s="1">
         <v>26.73</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="2">
         <f t="shared" si="0"/>
         <v>26.5866666666667</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="2">
         <f>F15-F18</f>
         <v>25.2133333333333</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="2">
         <f>((F15-F18)/F15)*100</f>
         <v>48.6743886743887</v>
       </c>
@@ -21440,15 +21435,15 @@
       <c r="E19" s="1">
         <v>26.84</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="2">
         <f t="shared" si="0"/>
         <v>26.5866666666667</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="2">
         <f>F15-F19</f>
         <v>25.2133333333333</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="2">
         <f>((F15-F19)/F15)*100</f>
         <v>48.6743886743887</v>
       </c>
@@ -21469,8 +21464,8 @@
   <sheetPr/>
   <dimension ref="B2:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="14.4"/>
@@ -21513,12 +21508,12 @@
       <c r="H4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="2:9">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C5" s="1">
@@ -21533,21 +21528,21 @@
       <c r="F5" s="1">
         <v>0.37</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="2">
         <f>SUM(D5:F5)/3</f>
         <v>0.35</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="2">
         <f>C5-G5</f>
         <v>-0.31</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <f>((C5-G5)/C5)*100</f>
         <v>-775</v>
       </c>
     </row>
     <row r="6" spans="2:9">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="1">
@@ -21562,21 +21557,21 @@
       <c r="F6" s="1">
         <v>0.75</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="2">
         <f>SUM(D6:F6)/3</f>
         <v>0.846666666666667</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="2">
         <f>C6-G6</f>
         <v>-0.596666666666667</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <f>((C6-G6)/C6)*100</f>
         <v>-238.666666666667</v>
       </c>
     </row>
     <row r="7" spans="2:9">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="1">
@@ -21591,21 +21586,21 @@
       <c r="F7" s="1">
         <v>2.68</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="2">
         <f>SUM(D7:F7)/3</f>
         <v>2.64333333333333</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="2">
         <f>C7-G7</f>
         <v>-0.623333333333333</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <f>((C7-G7)/C7)*100</f>
         <v>-30.8580858085808</v>
       </c>
     </row>
     <row r="8" spans="2:9">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C8" s="1">
@@ -21620,21 +21615,21 @@
       <c r="F8" s="1">
         <v>10.98</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="2">
         <f>SUM(D8:F8)/3</f>
         <v>11.0833333333333</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="2">
         <f>C8-G8</f>
         <v>4.50666666666667</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <f>((C8-G8)/C8)*100</f>
         <v>28.907419285867</v>
       </c>
     </row>
     <row r="9" spans="2:9">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="1">
@@ -21649,15 +21644,15 @@
       <c r="F9" s="1">
         <v>54.37</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="2">
         <f>SUM(D9:F9)/3</f>
         <v>54.62</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="2">
         <f>C9-G9</f>
         <v>67.75</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <f>((C9-G9)/C9)*100</f>
         <v>55.3648770123396</v>
       </c>
@@ -21695,32 +21690,32 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="2:7">
       <c r="B6" s="1" t="s">
@@ -21735,87 +21730,87 @@
       <c r="E6" s="1">
         <v>29.21</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <f>SUM(C6:E6)/3</f>
         <v>29.5166666666667</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>17.79</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>18.61</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>18.26</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <f>SUM(C7:E7)/3</f>
         <v>18.22</v>
       </c>
-      <c r="G7" s="3"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>20.63</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>19.97</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>20.88</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <f>SUM(C8:E8)/3</f>
         <v>20.4933333333333</v>
       </c>
-      <c r="G8" s="3"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>24.48</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>24.5</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>24.45</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <f>SUM(C9:E9)/3</f>
         <v>24.4766666666667</v>
       </c>
-      <c r="G9" s="3"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>27.09</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>27.21</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>26.98</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <f>SUM(C10:E10)/3</f>
         <v>27.0933333333333</v>
       </c>
-      <c r="G10" s="3"/>
+      <c r="G10" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -21832,8 +21827,8 @@
   <sheetPr/>
   <dimension ref="B3:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S38" sqref="S38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -21852,99 +21847,99 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="2:7">
       <c r="B7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>20.63</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>19.97</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>20.88</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <f>SUM(C7:E7)/3</f>
         <v>20.4933333333333</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>22.89</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>22.05</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>22.67</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <f>SUM(C8:E8)/3</f>
         <v>22.5366666666667</v>
       </c>
-      <c r="G8" s="3"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>